<commit_message>
MOD: Se modifico el README, aclarando que se necesita para correr el programa, por favorsito leer el README, me quedo algo bonito
</commit_message>
<xml_diff>
--- a/python/HistoricoEstudiEspe_output.xlsx
+++ b/python/HistoricoEstudiEspe_output.xlsx
@@ -7283,7 +7283,11 @@
           <t>1144063611</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr"/>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Vargas Cardona,Joan Sebastian</t>
+        </is>
+      </c>
       <c r="D92" t="n">
         <v>13</v>
       </c>

</xml_diff>